<commit_message>
Funcion exportar excel funcional
</commit_message>
<xml_diff>
--- a/src/ficheros/cursos.xlsx
+++ b/src/ficheros/cursos.xlsx
@@ -6,13 +6,56 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Curso 1" r:id="rId3" sheetId="1"/>
+    <sheet name="Cursos Intensivos" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t>Codigo Curso</t>
+  </si>
+  <si>
+    <t>Nombre Curso</t>
+  </si>
+  <si>
+    <t>Asistencia Minima</t>
+  </si>
+  <si>
+    <t>Relator</t>
+  </si>
+  <si>
+    <t>Alumno</t>
+  </si>
+  <si>
+    <t>Asistencia Alumno</t>
+  </si>
+  <si>
+    <t>Promedio Alumno</t>
+  </si>
+  <si>
+    <t>JAVA</t>
+  </si>
+  <si>
+    <t>Brayan</t>
+  </si>
+  <si>
+    <t>Nombre 1</t>
+  </si>
+  <si>
+    <t>Nombre 2</t>
+  </si>
+  <si>
+    <t>REACT</t>
+  </si>
+  <si>
+    <t>Nombre 3</t>
+  </si>
+  <si>
+    <t>nombre 5</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,18 +98,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="n" s="0">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
         <v>1.0</v>
       </c>
-      <c r="C1" t="n" s="0">
+      <c r="B2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>74.0</v>
+      </c>
+      <c r="G2" t="n" s="0">
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
         <v>2.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>5.333333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>